<commit_message>
added folder for clean csv and started cleaning
</commit_message>
<xml_diff>
--- a/Notes on sheet changes needed.xlsx
+++ b/Notes on sheet changes needed.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kyobu\Desktop\My Analysis Projects\electric outages\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kyobu\Desktop\My Analysis Projects\Maven_Power_Outage_Challenge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{315F13FA-E3EE-41A3-8914-78389AA2D88C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4070D6A-C0D5-4856-A32E-ADDC083FDFF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{EF41546C-488D-4A0F-91D9-0E3F8E822558}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="46">
   <si>
     <t>Header years</t>
   </si>
@@ -165,6 +165,15 @@
   </si>
   <si>
     <t>Added "Year" column</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>Deman Loss (MW)</t>
+  </si>
+  <si>
+    <t>Number of  Customers Affected</t>
   </si>
 </sst>
 </file>
@@ -542,14 +551,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B83B1A2-D423-45B1-812B-8F9957AB9DCA}">
-  <dimension ref="A1:N24"/>
+  <dimension ref="A1:N26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="2" max="2" width="15.36328125" customWidth="1"/>
     <col min="3" max="3" width="17.453125" customWidth="1"/>
     <col min="4" max="4" width="16.6328125" customWidth="1"/>
     <col min="5" max="5" width="18.453125" customWidth="1"/>
@@ -1379,6 +1389,38 @@
         <v>42</v>
       </c>
     </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>43</v>
+      </c>
+      <c r="B26" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" t="s">
+        <v>16</v>
+      </c>
+      <c r="D26" t="s">
+        <v>17</v>
+      </c>
+      <c r="E26" t="s">
+        <v>18</v>
+      </c>
+      <c r="F26" t="s">
+        <v>10</v>
+      </c>
+      <c r="G26" t="s">
+        <v>3</v>
+      </c>
+      <c r="H26" t="s">
+        <v>19</v>
+      </c>
+      <c r="I26" t="s">
+        <v>44</v>
+      </c>
+      <c r="J26" t="s">
+        <v>45</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:M2"/>

</xml_diff>

<commit_message>
cleaning sheets and converting to csv
</commit_message>
<xml_diff>
--- a/Notes on sheet changes needed.xlsx
+++ b/Notes on sheet changes needed.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kyobu\Desktop\My Analysis Projects\Maven_Power_Outage_Challenge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4070D6A-C0D5-4856-A32E-ADDC083FDFF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D3BB575-3E49-4888-B64F-B92124007722}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{EF41546C-488D-4A0F-91D9-0E3F8E822558}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="45">
   <si>
     <t>Header years</t>
   </si>
@@ -168,9 +168,6 @@
   </si>
   <si>
     <t>All</t>
-  </si>
-  <si>
-    <t>Deman Loss (MW)</t>
   </si>
   <si>
     <t>Number of  Customers Affected</t>
@@ -553,8 +550,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B83B1A2-D423-45B1-812B-8F9957AB9DCA}">
   <dimension ref="A1:N26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1415,10 +1412,10 @@
         <v>19</v>
       </c>
       <c r="I26" t="s">
+        <v>20</v>
+      </c>
+      <c r="J26" t="s">
         <v>44</v>
-      </c>
-      <c r="J26" t="s">
-        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changing folder name and updating notes sheet
</commit_message>
<xml_diff>
--- a/Notes on sheet changes needed.xlsx
+++ b/Notes on sheet changes needed.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kyobu\Desktop\My Analysis Projects\Maven_Power_Outage_Challenge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D3BB575-3E49-4888-B64F-B92124007722}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BA3C088-3AF6-4BFA-9523-E23F5C09D8B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{EF41546C-488D-4A0F-91D9-0E3F8E822558}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="58">
   <si>
     <t>Header years</t>
   </si>
@@ -101,9 +101,6 @@
     <t>Demand Loss (MW)</t>
   </si>
   <si>
-    <t>Culomn</t>
-  </si>
-  <si>
     <t>A</t>
   </si>
   <si>
@@ -171,6 +168,48 @@
   </si>
   <si>
     <t>Number of  Customers Affected</t>
+  </si>
+  <si>
+    <t>Column</t>
+  </si>
+  <si>
+    <t>Header Column Names</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>I treated as a 0 value (no one affected)</t>
+  </si>
+  <si>
+    <t>"500-600"</t>
+  </si>
+  <si>
+    <t>on ranges like example, I chose the higher number</t>
+  </si>
+  <si>
+    <t>"under" or "over"</t>
+  </si>
+  <si>
+    <t>I selected the number given</t>
+  </si>
+  <si>
+    <t>How I treated NA, ranges, nonspecific, or no data:</t>
+  </si>
+  <si>
+    <t>Unknown</t>
+  </si>
+  <si>
+    <t>no report of restoration</t>
+  </si>
+  <si>
+    <t>no time given (e.g. "Evening)</t>
+  </si>
+  <si>
+    <t>If no restoration time, gave 9:00 p.m.</t>
+  </si>
+  <si>
+    <t>In Demand and customers affected, set at 0</t>
   </si>
 </sst>
 </file>
@@ -548,14 +587,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B83B1A2-D423-45B1-812B-8F9957AB9DCA}">
-  <dimension ref="A1:N26"/>
+  <dimension ref="A1:N35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="1" max="1" width="43.08984375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.36328125" customWidth="1"/>
     <col min="3" max="3" width="17.453125" customWidth="1"/>
     <col min="4" max="4" width="16.6328125" customWidth="1"/>
@@ -573,46 +613,46 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" t="s">
         <v>21</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>22</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>23</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>24</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>25</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>26</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>27</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>28</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>29</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>30</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>31</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>32</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>33</v>
-      </c>
-      <c r="N1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="29" x14ac:dyDescent="0.35">
@@ -692,7 +732,7 @@
         <v>13</v>
       </c>
       <c r="N4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
@@ -782,7 +822,7 @@
         <v>12</v>
       </c>
       <c r="N7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
@@ -843,7 +883,7 @@
         <v>13</v>
       </c>
       <c r="N9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
@@ -936,7 +976,7 @@
         <v>8</v>
       </c>
       <c r="N12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
@@ -1040,7 +1080,7 @@
         <v>2015</v>
       </c>
       <c r="B16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C16" t="s">
         <v>15</v>
@@ -1061,7 +1101,7 @@
         <v>3</v>
       </c>
       <c r="I16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J16" t="s">
         <v>19</v>
@@ -1073,7 +1113,7 @@
         <v>8</v>
       </c>
       <c r="N16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.35">
@@ -1081,7 +1121,7 @@
         <v>2016</v>
       </c>
       <c r="B17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C17" t="s">
         <v>15</v>
@@ -1102,7 +1142,7 @@
         <v>3</v>
       </c>
       <c r="I17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J17" t="s">
         <v>19</v>
@@ -1119,7 +1159,7 @@
         <v>2017</v>
       </c>
       <c r="B18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C18" t="s">
         <v>15</v>
@@ -1140,7 +1180,7 @@
         <v>3</v>
       </c>
       <c r="I18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J18" t="s">
         <v>19</v>
@@ -1157,7 +1197,7 @@
         <v>2018</v>
       </c>
       <c r="B19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C19" t="s">
         <v>15</v>
@@ -1178,7 +1218,7 @@
         <v>3</v>
       </c>
       <c r="I19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J19" t="s">
         <v>19</v>
@@ -1195,7 +1235,7 @@
         <v>2019</v>
       </c>
       <c r="B20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C20" t="s">
         <v>15</v>
@@ -1216,7 +1256,7 @@
         <v>3</v>
       </c>
       <c r="I20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J20" t="s">
         <v>19</v>
@@ -1233,7 +1273,7 @@
         <v>2020</v>
       </c>
       <c r="B21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C21" t="s">
         <v>15</v>
@@ -1254,7 +1294,7 @@
         <v>3</v>
       </c>
       <c r="I21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J21" t="s">
         <v>19</v>
@@ -1271,7 +1311,7 @@
         <v>2021</v>
       </c>
       <c r="B22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C22" t="s">
         <v>15</v>
@@ -1292,7 +1332,7 @@
         <v>3</v>
       </c>
       <c r="I22" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J22" t="s">
         <v>19</v>
@@ -1309,7 +1349,7 @@
         <v>2022</v>
       </c>
       <c r="B23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C23" t="s">
         <v>15</v>
@@ -1330,7 +1370,7 @@
         <v>3</v>
       </c>
       <c r="I23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J23" t="s">
         <v>19</v>
@@ -1347,10 +1387,10 @@
         <v>2023</v>
       </c>
       <c r="B24" t="s">
+        <v>39</v>
+      </c>
+      <c r="C24" t="s">
         <v>40</v>
-      </c>
-      <c r="C24" t="s">
-        <v>41</v>
       </c>
       <c r="D24" t="s">
         <v>15</v>
@@ -1371,7 +1411,7 @@
         <v>3</v>
       </c>
       <c r="J24" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K24" t="s">
         <v>19</v>
@@ -1383,39 +1423,94 @@
         <v>8</v>
       </c>
       <c r="N24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>42</v>
+      </c>
+      <c r="B27" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" t="s">
+        <v>16</v>
+      </c>
+      <c r="D27" t="s">
+        <v>17</v>
+      </c>
+      <c r="E27" t="s">
+        <v>18</v>
+      </c>
+      <c r="F27" t="s">
+        <v>10</v>
+      </c>
+      <c r="G27" t="s">
+        <v>3</v>
+      </c>
+      <c r="H27" t="s">
+        <v>19</v>
+      </c>
+      <c r="I27" t="s">
+        <v>20</v>
+      </c>
+      <c r="J27" t="s">
         <v>43</v>
       </c>
-      <c r="B26" t="s">
-        <v>15</v>
-      </c>
-      <c r="C26" t="s">
-        <v>16</v>
-      </c>
-      <c r="D26" t="s">
-        <v>17</v>
-      </c>
-      <c r="E26" t="s">
-        <v>18</v>
-      </c>
-      <c r="F26" t="s">
-        <v>10</v>
-      </c>
-      <c r="G26" t="s">
-        <v>3</v>
-      </c>
-      <c r="H26" t="s">
-        <v>19</v>
-      </c>
-      <c r="I26" t="s">
-        <v>20</v>
-      </c>
-      <c r="J26" t="s">
-        <v>44</v>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>46</v>
+      </c>
+      <c r="B30" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>48</v>
+      </c>
+      <c r="B31" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>50</v>
+      </c>
+      <c r="B32" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>53</v>
+      </c>
+      <c r="B33" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>55</v>
+      </c>
+      <c r="B35" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>